<commit_message>
get the base in, small update to rough plan
</commit_message>
<xml_diff>
--- a/Rough Plan.xlsx
+++ b/Rough Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Info" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Nathan Rooke</t>
   </si>
@@ -60,9 +60,6 @@
     <t>move =&gt;</t>
   </si>
   <si>
-    <t>One main class which everything will inherit from. It can be called something like 'PacObject'. This will be the object type of our 2 dimensional array. PacObject will have a 'move' method. Also some kind of hit detection.</t>
-  </si>
-  <si>
     <t>pacPrize inherits PacObject</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Iteration 5 (optional)</t>
   </si>
   <si>
-    <t>Randomally the map</t>
-  </si>
-  <si>
     <t>Ghost movement algorithms: mirrors your movements, djirksta's alg, random movments, teleporty</t>
   </si>
   <si>
@@ -103,6 +97,21 @@
   </si>
   <si>
     <t>drewmichel33@gmail.com</t>
+  </si>
+  <si>
+    <t>661 809 6224</t>
+  </si>
+  <si>
+    <t>Randomally generate the map</t>
+  </si>
+  <si>
+    <t>PacWall inherits PacObject</t>
+  </si>
+  <si>
+    <t>One main class which everything will inherit from. It can be called something like 'PacObject'. This will be the object type of our 2 dimensional array. PacObject will have a 'move' method. It's current x,y location (might not need this). Also some kind of detectHit method. We also need some sort of logic over what would 'win' in a collision. e.g. PacMan eats PacPrize but PacEnemy eats PacMan. Plus account for PacWall.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since we're doing array based collisions we need to determine some kind of central clock for managing movements. </t>
   </si>
 </sst>
 </file>
@@ -470,18 +479,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="C33:D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,23 +501,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>6618096224</v>
+      <c r="B2" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -524,64 +533,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.9296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="52.46484375" customWidth="1"/>
+    <col min="1" max="1" width="69" style="2" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="57" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -597,49 +616,49 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -651,30 +670,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49:F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.9296875" customWidth="1"/>
-    <col min="3" max="3" width="2.265625" customWidth="1"/>
-    <col min="5" max="5" width="1.86328125" customWidth="1"/>
-    <col min="7" max="7" width="1.73046875" customWidth="1"/>
-    <col min="9" max="9" width="1.86328125" customWidth="1"/>
+    <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" ht="40.15" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="3" ht="9.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="4" ht="44.65" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="5" ht="9.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="6" ht="45.75" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="7" ht="7.5" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="8" ht="44.65" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="9" ht="9.4" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="10" ht="48" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="11" ht="9" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" ht="9.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" ht="44.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" ht="9.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" ht="44.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" ht="9.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
@Julian Conner Added plan to use and change move algorithms at runtime in plan
Added my phone numbers and email in the contact info.
</commit_message>
<xml_diff>
--- a/Rough Plan.xlsx
+++ b/Rough Plan.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Info" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Iterations" sheetId="3" r:id="rId3"/>
     <sheet name="Map" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Nathan Rooke</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Andrew Michel</t>
   </si>
   <si>
-    <t>Julian Connor</t>
-  </si>
-  <si>
     <t>Zachary Pwell</t>
   </si>
   <si>
@@ -112,6 +109,92 @@
   </si>
   <si>
     <t xml:space="preserve">Since we're doing array based collisions we need to determine some kind of central clock for managing movements. </t>
+  </si>
+  <si>
+    <t>Julian Conner</t>
+  </si>
+  <si>
+    <t>juconner@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @ By : Julian Conner
+- Could have a Moveable interface that each
+moving Entity/PacObject implements. The interface
+would have a moveObject() method. 
+   - This way we don't need to check or store
+    instance variables to see if the object can move
+   because all functions in our program that cause
+   the Entity/PacObject to move will just look for
+   a Moveable  object type. This guarentees that
+   the object has the ability to move without getting
+  into complicated specifics about the specific class
+  or values its instance variables has. 
+-The implementing class will have a Strategy object
+(see definition below ) perform its action in the
+implemented moveObject() method. The different
+algorithms will be in it's own Strategy object, which
+we can set and swap with other Strategy objects as
+we wish at runtime. The Strategy object can hold
+a reference of the object it's changing as an
+instance variable.
+Strategy Object Definition :
+( an object that holds an algorithm or type of action ,
+ which can be switched out at runtime with other 
+Strategy objects that use a different algorithm or
+ way to perform the same function call )
+Strategy Pattern - allows you to change algorithms
+and implementations of the same object's actions
+at runtime by changing the object's Strategy object
+instance variable as described above.
+ - Use Strategy Pattern to change
+the movement algorithm during runtime. Could have
+a MoveStrategy interface with a move() method,
+ then each movement algorithm will have its 
+own concrete class that implements the
+MoveStrategy interface.
+    - this way we can have the object who's moving only
+     need to worry about having a MoveStrategy instance
+   instance variable because all the subclasses are that
+  type. We won't need to worry about which specific
+   subclass it is because its guaranteed we'll be able to use them the
+  same.
+- Each subclass will implement the move() method using the algorithm
+the class represents. Each subclass will have an
+instance variable that is a Moveable object. This way we dont' have
+to worry about which specific moving PacObject it is, we only worry
+about if it the object can move. The implementation of the move() method will
+manipulate the Moveable object (ex: pacman or
+the enemies ).
+-If there are specific values the moving object needs to modify
+  when it is moved on the game board, then we can make an interface
+  (MovablePacObject) that has methods to get , set, and process them, then we could make
+PacMan and his enemies implement it.
+    - Instead of using the Moveable type as the Strategy method's instance variable
+       we can make it store a MovablePacObject instance variable to modifiy
+      when move() is called.
+It's open to modification :
+As we further plan this out, we can decide whether or not to pass
+data into the move() or moveObject() methods if it turns out our
+program needs to.
+- Could pass an Object that has all the data we need
+  - if the Pacman move() algorithm requires different data than the
+   enemies algorithm then this would be a better choice because 
+   we can put the data Pacman and the enemies need in the same
+  type of object, which each Strategy class's implementation will
+   take the data it actually needs, and the fact that it uses the same
+   object type, both the Strategy class and the Moveable PacObject
+  classes still only need to implement that same interface and method,
+  otherwise we would need to make multiple move methods for the
+  PacObject's and Strategy objects.
+    - we could pass in the user's key inputs if needed, etc.
+- Could pass values in directly but is less flexible
+</t>
+  </si>
+  <si>
+    <t>(main phone) : 
+760 791 6633
+ (iTouch, only works when there's wifi ) :
+ 760 491 7187</t>
   </si>
 </sst>
 </file>
@@ -156,12 +239,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -479,18 +572,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="C33:D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.5546875" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,31 +594,38 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -533,78 +633,503 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="69" style="2" customWidth="1"/>
-    <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.44140625" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:F74"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -616,49 +1141,49 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -674,26 +1199,26 @@
       <selection activeCell="F49" sqref="F49:F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="3" max="3" width="2.28515625" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" customWidth="1"/>
-    <col min="9" max="9" width="1.85546875" customWidth="1"/>
+    <col min="3" max="3" width="2.33203125" customWidth="1"/>
+    <col min="5" max="5" width="1.88671875" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" customWidth="1"/>
+    <col min="9" max="9" width="1.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" ht="40.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" ht="9.4" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" ht="44.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" ht="9.4" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" ht="44.65" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" ht="9.4" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" ht="48" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" ht="40.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" ht="44.7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="6" ht="45.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" ht="44.7" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" ht="48" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" ht="9" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>